<commit_message>
Bloqueo Guión CS_06_01_CO y CS_08_01_CO
</commit_message>
<xml_diff>
--- a/seguimiento/ProduccionDigital/SegDigital_CS_06_01_CO.xlsx
+++ b/seguimiento/ProduccionDigital/SegDigital_CS_06_01_CO.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\CienciasSociales\seguimiento\ProduccionDigital\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21713" windowHeight="9711"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21720" windowHeight="9720"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -220,9 +218,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +273,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -312,24 +326,26 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -349,35 +365,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -436,7 +457,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,7 +492,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -648,7 +669,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -660,28 +681,28 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G27" sqref="G27"/>
+      <selection pane="topRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="7.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.73046875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.53125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" style="1" customWidth="1"/>
-    <col min="5" max="8" width="12.06640625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.6640625" style="1"/>
+    <col min="1" max="1" width="7.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="1" customWidth="1"/>
+    <col min="5" max="8" width="12" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.100000000000001" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:15" ht="18">
+      <c r="A1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" ht="21.15" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:15" s="2" customFormat="1" ht="22">
       <c r="A3" s="4" t="s">
         <v>23</v>
       </c>
@@ -724,547 +745,598 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" ht="15.85" x14ac:dyDescent="0.45">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:15" ht="15">
+      <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="15"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="14">
         <v>42087.62777777778</v>
       </c>
-      <c r="F4" s="10">
+      <c r="F4" s="14">
         <v>42087.663194444445</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A5" s="13" t="s">
+      <c r="H4" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A6" s="13" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A7" s="13" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A8" s="13" t="s">
+      <c r="C7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="9" t="s">
+      <c r="C8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A9" s="13" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A10" s="13" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="C10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A11" s="13" t="s">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A12" s="13" t="s">
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="10"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A13" s="13" t="s">
+      <c r="C12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="9" t="s">
+      <c r="C13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="10"/>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A14" s="13" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="10"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A15" s="13" t="s">
+      <c r="C14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C15" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="9" t="s">
+      <c r="C15" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="10"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A16" s="13" t="s">
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="9" t="s">
+      <c r="C16" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="10"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="13" t="s">
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I16" s="9"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="13" t="s">
+      <c r="C17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="10"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="13" t="s">
+      <c r="C18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="10"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="13" t="s">
+      <c r="C19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="9" t="s">
+      <c r="C20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="10"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="13" t="s">
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="10"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="13" t="s">
+      <c r="C21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="10"/>
-    </row>
-    <row r="23" spans="1:13" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="A23" s="13" t="s">
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:13" ht="24">
+      <c r="A23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="10"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A24" s="13" t="s">
+      <c r="C23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="A24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C24" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="10"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A25" s="13" t="s">
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="14"/>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="10"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A26" s="13" t="s">
+      <c r="C25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="A26" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="10"/>
+      <c r="C26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="16">
+        <v>42088.333333333336</v>
+      </c>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="L4:L26"/>
     <mergeCell ref="M4:M26"/>
     <mergeCell ref="E4:E26"/>
     <mergeCell ref="F4:F26"/>
     <mergeCell ref="G4:G26"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>